<commit_message>
calistir ve form kısımları ayrı dosyalara alındı ufak tefek kontroller gerçekleştirildi
</commit_message>
<xml_diff>
--- a/bodyDataBase.xlsx
+++ b/bodyDataBase.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
   <si>
     <t xml:space="preserve">
 window._sharedData = {"activity_counts":null,"config":{"csrf_token":"vgHMliGwF9FeEcv33pPkR4Stb0twHC6D","viewer":null},"country_code":"DE","language_code":"en","locale":"en_US","entry_data":{"ProfilePage":[{"user":{"biography":"\u003c\u003c\u003c\u003cComputer Engineer\u003e\u003e\u003e\u003e\n     MPAL \u0026 SA\u00dc Graduated\n              Bursa \u2708\ufe0f Berlin\n                    Archer \n______________\ud83c\uddf9\ud83c\uddf7_____________","blocked_by_viewer":false,"country_block":false,"external_url":null,"external_url_linkshimmed":null,"followed_by":{"count":541},"followed_by_viewer":false,"follows":{"count":291},"follows_viewer":false,"full_name":"____________\u003cTK\u003e____________","has_blocked_viewer":false,"has_requested_viewer":false,"id":"1700499581","is_private":true,"is_verified":false,"mutual_followers":null,"profile_pic_url":"https://scontent-frt3-2.cdninstagram.com/vp/ae8cca32468cae276fd70a823898fcc1/5B28BE4A/t51.2885-19/s150x150/26866731_836251886546942_8991696596055883776_n.jpg","profile_pic_url_hd":"https://scontent-frt3-2.cdninstagram.com/vp/e53ac13652c0e170cd623c31c3e73385/5B18ABBA/t51.2885-19/s320x320/26866731_836251886546942_8991696596055883776_n.jpg","requested_by_viewer":false,"username":"tlgkyck","connected_fb_page":null,"media":{"nodes":[],"count":208,"page_info":{"has_next_page":true,"end_cursor":"AQA68Sfd3Qz-l1_4JiLtYYrX_fxAyYIGb2kJt7DppWxHaGEkPwcGL8lJUqXQGjRCNpSmUNY55TuAU-HuR6k0EL40xj_W70vo-vOXq4AixRfzVw"}},"saved_media":{"nodes":[],"count":0,"page_info":{"has_next_page":false,"end_cursor":null}},"media_collections":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]}},"logging_page_id":"profilePage_1700499581","show_suggested_profiles":false,"graphql":{"user":{"biography":"\u003c\u003c\u003c\u003cComputer Engineer\u003e\u003e\u003e\u003e\n     MPAL \u0026 SA\u00dc Graduated\n              Bursa \u2708\ufe0f Berlin\n                    Archer \n______________\ud83c\uddf9\ud83c\uddf7_____________","blocked_by_viewer":false,"country_block":false,"external_url":null,"external_url_linkshimmed":null,"edge_followed_by":{"count":541},"followed_by_viewer":false,"edge_follow":{"count":291},"follows_viewer":false,"full_name":"____________\u003cTK\u003e____________","has_blocked_viewer":false,"has_requested_viewer":false,"id":"1700499581","is_private":true,"is_verified":false,"mutual_followers":null,"profile_pic_url":"https://scontent-frt3-2.cdninstagram.com/vp/ae8cca32468cae276fd70a823898fcc1/5B28BE4A/t51.2885-19/s150x150/26866731_836251886546942_8991696596055883776_n.jpg","profile_pic_url_hd":"https://scontent-frt3-2.cdninstagram.com/vp/e53ac13652c0e170cd623c31c3e73385/5B18ABBA/t51.2885-19/s320x320/26866731_836251886546942_8991696596055883776_n.jpg","requested_by_viewer":false,"username":"tlgkyck","connected_fb_page":null,"edge_owner_to_timeline_media":{"count":208,"page_info":{"has_next_page":true,"end_cursor":"AQA68Sfd3Qz-l1_4JiLtYYrX_fxAyYIGb2kJt7DppWxHaGEkPwcGL8lJUqXQGjRCNpSmUNY55TuAU-HuR6k0EL40xj_W70vo-vOXq4AixRfzVw"},"edges":[]},"edge_saved_media":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]},"edge_media_collections":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]}}}}]},"gatekeepers":{"ld":true,"seo":true},"qe":{"client_gql":{"g":"","p":{}},"dash_for_vod":{"g":"","p":{}},"bc3l":{"g":"","p":{}},"aysf":{"g":"","p":{}},"notif":{"g":"","p":{}},"follow_button":{"g":"","p":{}},"loggedout":{"g":"launch","p":{"new_cta":"true","remove_upsell_banner":"true","update_nav":"true"}},"loggedout_upsell":{"g":"","p":{}},"stories":{"g":"","p":{}},"exit_story_creation":{"g":"","p":{}},"su_universe":{"g":"test_msisdn_prefill_12_18","p":{"has_msisdn_prefill":"true"}},"us_li":{"g":"","p":{}},"sidecar":{"g":"","p":{}},"video":{"g":"","p":{}},"appsell":{"g":"","p":{}},"collections":{"g":"","p":{}},"msisdn":{"g":"test_prefill_2_15","p":{"has_msisdn_prefill":"true"}},"save":{"g":"","p":{}},"stale":{"g":"","p":{}},"reg":{"g":"control_inline_2_01_16","p":{"has_inline_labels":"false"}},"reg_vp":{"g":"test_group_1","p":{"hide_value_prop":"true"}},"prof_pic_upsell":{"g":"","p":{}},"prof_pic_creation":{"g":"","p":{}},"onetaplogin":{"g":"","p":{}},"onetaplogin_userbased":{"g":"","p":{}},"feed_vp":{"g":"","p":{}},"push_notifications":{"g":"","p":{}},"login_poe":{"g":"","p":{}},"report_haf":{"g":"","p":{}},"report_profile":{"g":"","p":{}},"reporting":{"g":"","p":{}},"media_reporting":{"g":"","p":{}},"bg_sync":{"g":"","p":{}},"disc_ppl":{"g":"","p":{}},"ebdsim_li":{"g":"","p":{}},"ebdsim_lo":{"g":"","p":{}},"embeds":{"g":"","p":{}},"prvcy_tggl":{"g":"","p":{}},"tp_pblshr":{"g":"","p":{}},"fs":{"g":"","p":{}},"404_as_react":{"g":"","p":{}},"acc_recovery":{"g":"","p":{}},"connections":{"g":"","p":{}}},"hostname":"www.instagram.com","display_properties_server_guess":{"pixel_ratio":1.5,"viewport_width":360,"viewport_height":480,"orientation":""},"environment_switcher_visible_server_guess":true,"platform":"web","nonce":"k05odc1FHtEW7COQpskzNQ==","zero_data":{},"is_canary":true,"rollout_hash":"5382794631a5","probably_has_app":false,"show_app_install":true};
@@ -810,6 +810,89 @@
 fbq('init', '1425767024389221');
 fbq('track', 'PageView');
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+								Serdar YILMAZ								
+								Bizimkisi Bir “Bug” Hikayesi...							
+ Serdivan/Sakarya						
+ iletisim@srdrylmz.com							
+ Serdar Yılmaz  Ana Sayfa						
+Son Yazılar
+							Tüm Yazıları Görün ››
+Kas.
+29
+2017
+									Biyoteknolojiye Hazır mıyız?								
+Büyük bir merakla takip ettiğim biyoteknoloji alanındaki gelişmeleri bu içerikte toparlayıp; biyoteknolojinin ne olduğuna, bu alanda yapılan çalışmalara, yatırımlara ve gelecekte karşılaşabileceğimiz olası senaryolara değinmeye çalışacağım. Devamını Okumak İçin Tıklayınız…
+Haz.
+03
+2017
+									Yaşam İçin Anlam Taşıyan Üç Şey								
+Bu yazıda, Linux’un yaratıcısı Linus Torvalds’ın bilgisayar dünyasına girişini konu alan “Yalnızca Eğlenmek İçin” isimli kitaptan bir bölüme yer vereceğim. Kitabı yaklaşık 1 – 1.5 yıl önce okumuştum, bugün kitaplığı düzenlerken görünce altını çizdiğim kısımlara tekrar göz gezdirdim ve bir kısmını blog da paylaşmaya karar verdim. Linus Torvalds tarafından kaleme alınan ve onun fikirlerini, düşüncelerini, bakış açısını içeren bu kitabı okumanızı tavsiye ederim.  Devamını Okumak İçin Tıklayınız…
+Mar.
+05
+2017
+									Yaşamınızdaki Öncelikler Nedir ?								
+Bu yazıda Beyaz Yaka Kitap Kulübünün şubat ayı abonelerine göndermiş olduğu 4 kitaptan biri olan “Konuşmayı Kes Harekete Geç” isimli kitaptan bir alıntıya yer vereceğim. Her ne kadar kitabı sıkıcı bulup, sonlara doğru göz ucuyla okumuş olsam da kitabın ilk sayfasında yer alan öykü ilgimi çekti. Kitabı sıkıcı bulmamın nedeni bu tarz içeriklerin artık bende belli bir duygunluğa ulaşmasından kaynaklanıyor olabilir. Çünkü anlatılmak istenenler bir noktadan sonra sıradanlaşmaya başlayıp, tekrara düşüyor.  Devamını Okumak İçin Tıklayınız…
+Oca.
+19
+2017
+									C# – Koleksiyonlar								
+Nesne yönelimli programlama ile birlikte sınıf(class) kavramıyla tanıştık ve sıkça kullandığımız metotları tekrar tekrar yazmak yerine, bir sınıf içerisinde, bir defaya mahsus yazarak kod kalabalığının önüne geçmiş olduk. Bu programcı olarak bizlerin, kod karmaşıklığını ve kalabalığını azaltmaya yönelik olarak kendimizce almış olduğumuz bir önlem. Kullanmış olduğumuz platformda, programcılar tarafından sıkça kullanılan veri yapılarını hazır bir şekilde sunarak, benzeri bir kolaylık sağlamakta. Devamını Okumak İçin Tıklayınız…
+Oca.
+12
+2017
+									Kitap: Satranç – Stefan Zweig								
+Kitaptan bahsetmeye başlamadan önce Türkiye İş Bankası Kültür Yayınları hakkında kısaca bilgi vermek istiyorum. Türkiye İş Bankası Kültür Yayınları dünya klasiklerini dilimize kazandırmak amacıyla kurulan ülkemizdeki en köklü yayın evlerinden biri. Yayın evi hakkında özellikle değinmek istediğim nokta, kitapları bir dizi haline getirmiş olması. Stefan Zweig kaleme aldığı Satranç isimli kitapta, yayın evi tarafından oluşturulan Modern Klasikler Dizisi içerisinde yer almakta.  Devamını Okumak İçin Tıklayınız…
+Eyl.
+24
+2016
+									Kitap: Dijital Kale – Dan Brown								
+Şuana kadar Dan Brown’un Robert Langdon serisinden Melekler ve Şeytanlar, Da Vinci Şifresi ve Cehennem isimli kitaplarını okuyabildim. Seri içerisinde okumadığım sadece Kayıp Sembol kaldı. Aslında Kayıp Sembole başlangıç yapmıştım ancak vizeler başlayınca uzun bir süre okuyamadım. Bu yüzden kaldığım yerden devam etmek yerine, kitabı bir köşeye koyup farklı bir kitaba başlamayı tercih ettim. Dan Brown’un kaleme aldığı romanları okuyan arkadaşlar bu durumu anlayacaktır. Genellikle kitapları ortalayıncaya kadar olaylar oldukça durgun bir seyir izlemekte. Sanırım kitabı yeniden okumama nedenimde bu; okuduğum kısımları tekrar okumak zorunda kalmam ve bu kısımların durgun ilerlemesi. Devamını Okumak İçin Tıklayınız…
+Ana Sayfa
+Blog
+Genel
+Kodlama
+Teknoloji
+Alıntılar
+Faydalı Siteler
+İnternet
+Kitap &amp; Dergi
+Etkinlikler
+Hakkımda
+Multimedya
+				© Copyright 2013. All Rights Reserved.			
+				Serdar YILMAZ Kişisel Web Günlüğü			
+    (function (d, w, c) {
+        (w[c] = w[c] || []).push(function() {
+            try {
+                w.yaCounter35156325 = new Ya.Metrika({
+                    id:35156325,
+                    clickmap:true,
+                    trackLinks:true,
+                    accurateTrackBounce:true,
+                    webvisor:true
+                });
+            } catch(e) { }
+        });
+        var n = d.getElementsByTagName("script")[0],
+            s = d.createElement("script"),
+            f = function () { n.parentNode.insertBefore(s, n); };
+        s.type = "text/javascript";
+        s.async = true;
+        s.src = "https://mc.yandex.ru/metrika/watch.js";
+        if (w.opera == "[object Opera]") {
+            d.addEventListener("DOMContentLoaded", f, false);
+        } else { f(); }
+    })(document, window, "yandex_metrika_callbacks");
+/* &lt;![CDATA[ */
+var JQLBSettings = {"fitToScreen":"1","resizeSpeed":"400","displayDownloadLink":"0","navbarOnTop":"0","loopImages":"","resizeCenter":"","marginSize":"0","linkTarget":"","help":"","prevLinkTitle":"previous image","nextLinkTitle":"next image","prevLinkText":"\u00ab Previous","nextLinkText":"Next \u00bb","closeTitle":"close image gallery","image":"Image ","of":" of ","download":"Download","jqlb_overlay_opacity":"80","jqlb_overlay_color":"#000000","jqlb_overlay_close":"1","jqlb_border_width":"10","jqlb_border_color":"#ffffff","jqlb_border_radius":"0","jqlb_image_info_background_transparency":"100","jqlb_image_info_bg_color":"#ffffff","jqlb_image_info_text_color":"#000000","jqlb_image_info_text_fontsize":"10","jqlb_show_text_for_image":"1","jqlb_next_image_title":"next image","jqlb_previous_image_title":"previous image","jqlb_next_button_image":"http:\/\/www.srdrylmz.com\/wp-content\/plugins\/wp-lightbox-2\/styles\/images\/next.gif","jqlb_previous_button_image":"http:\/\/www.srdrylmz.com\/wp-content\/plugins\/wp-lightbox-2\/styles\/images\/prev.gif","jqlb_maximum_width":"","jqlb_maximum_height":"","jqlb_show_close_button":"1","jqlb_close_image_title":"close image gallery","jqlb_close_image_max_heght":"22","jqlb_image_for_close_lightbox":"http:\/\/www.srdrylmz.com\/wp-content\/plugins\/wp-lightbox-2\/styles\/images\/closelabel.gif","jqlb_keyboard_navigation":"1","jqlb_popup_size_fix":"0"};
+/* ]]&gt; */
+</t>
+  </si>
+  <si>
+    <t>http://www.srdrylmz.com/</t>
   </si>
 </sst>
 </file>
@@ -1150,7 +1233,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z56"/>
+  <dimension ref="A1:Z57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
@@ -1780,6 +1863,17 @@
         <v>47</v>
       </c>
     </row>
+    <row r="57" spans="1:26">
+      <c r="A57" s="2" t="n">
+        <v>43157.5274284332</v>
+      </c>
+      <c r="C57" t="s">
+        <v>59</v>
+      </c>
+      <c r="I57" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Girdiler form ekranına alındı bootstrap eklendi
</commit_message>
<xml_diff>
--- a/bodyDataBase.xlsx
+++ b/bodyDataBase.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
   <si>
     <t xml:space="preserve">
 window._sharedData = {"activity_counts":null,"config":{"csrf_token":"vgHMliGwF9FeEcv33pPkR4Stb0twHC6D","viewer":null},"country_code":"DE","language_code":"en","locale":"en_US","entry_data":{"ProfilePage":[{"user":{"biography":"\u003c\u003c\u003c\u003cComputer Engineer\u003e\u003e\u003e\u003e\n     MPAL \u0026 SA\u00dc Graduated\n              Bursa \u2708\ufe0f Berlin\n                    Archer \n______________\ud83c\uddf9\ud83c\uddf7_____________","blocked_by_viewer":false,"country_block":false,"external_url":null,"external_url_linkshimmed":null,"followed_by":{"count":541},"followed_by_viewer":false,"follows":{"count":291},"follows_viewer":false,"full_name":"____________\u003cTK\u003e____________","has_blocked_viewer":false,"has_requested_viewer":false,"id":"1700499581","is_private":true,"is_verified":false,"mutual_followers":null,"profile_pic_url":"https://scontent-frt3-2.cdninstagram.com/vp/ae8cca32468cae276fd70a823898fcc1/5B28BE4A/t51.2885-19/s150x150/26866731_836251886546942_8991696596055883776_n.jpg","profile_pic_url_hd":"https://scontent-frt3-2.cdninstagram.com/vp/e53ac13652c0e170cd623c31c3e73385/5B18ABBA/t51.2885-19/s320x320/26866731_836251886546942_8991696596055883776_n.jpg","requested_by_viewer":false,"username":"tlgkyck","connected_fb_page":null,"media":{"nodes":[],"count":208,"page_info":{"has_next_page":true,"end_cursor":"AQA68Sfd3Qz-l1_4JiLtYYrX_fxAyYIGb2kJt7DppWxHaGEkPwcGL8lJUqXQGjRCNpSmUNY55TuAU-HuR6k0EL40xj_W70vo-vOXq4AixRfzVw"}},"saved_media":{"nodes":[],"count":0,"page_info":{"has_next_page":false,"end_cursor":null}},"media_collections":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]}},"logging_page_id":"profilePage_1700499581","show_suggested_profiles":false,"graphql":{"user":{"biography":"\u003c\u003c\u003c\u003cComputer Engineer\u003e\u003e\u003e\u003e\n     MPAL \u0026 SA\u00dc Graduated\n              Bursa \u2708\ufe0f Berlin\n                    Archer \n______________\ud83c\uddf9\ud83c\uddf7_____________","blocked_by_viewer":false,"country_block":false,"external_url":null,"external_url_linkshimmed":null,"edge_followed_by":{"count":541},"followed_by_viewer":false,"edge_follow":{"count":291},"follows_viewer":false,"full_name":"____________\u003cTK\u003e____________","has_blocked_viewer":false,"has_requested_viewer":false,"id":"1700499581","is_private":true,"is_verified":false,"mutual_followers":null,"profile_pic_url":"https://scontent-frt3-2.cdninstagram.com/vp/ae8cca32468cae276fd70a823898fcc1/5B28BE4A/t51.2885-19/s150x150/26866731_836251886546942_8991696596055883776_n.jpg","profile_pic_url_hd":"https://scontent-frt3-2.cdninstagram.com/vp/e53ac13652c0e170cd623c31c3e73385/5B18ABBA/t51.2885-19/s320x320/26866731_836251886546942_8991696596055883776_n.jpg","requested_by_viewer":false,"username":"tlgkyck","connected_fb_page":null,"edge_owner_to_timeline_media":{"count":208,"page_info":{"has_next_page":true,"end_cursor":"AQA68Sfd3Qz-l1_4JiLtYYrX_fxAyYIGb2kJt7DppWxHaGEkPwcGL8lJUqXQGjRCNpSmUNY55TuAU-HuR6k0EL40xj_W70vo-vOXq4AixRfzVw"},"edges":[]},"edge_saved_media":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]},"edge_media_collections":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]}}}}]},"gatekeepers":{"ld":true,"seo":true},"qe":{"client_gql":{"g":"","p":{}},"dash_for_vod":{"g":"","p":{}},"bc3l":{"g":"","p":{}},"aysf":{"g":"","p":{}},"notif":{"g":"","p":{}},"follow_button":{"g":"","p":{}},"loggedout":{"g":"launch","p":{"new_cta":"true","remove_upsell_banner":"true","update_nav":"true"}},"loggedout_upsell":{"g":"","p":{}},"stories":{"g":"","p":{}},"exit_story_creation":{"g":"","p":{}},"su_universe":{"g":"test_msisdn_prefill_12_18","p":{"has_msisdn_prefill":"true"}},"us_li":{"g":"","p":{}},"sidecar":{"g":"","p":{}},"video":{"g":"","p":{}},"appsell":{"g":"","p":{}},"collections":{"g":"","p":{}},"msisdn":{"g":"test_prefill_2_15","p":{"has_msisdn_prefill":"true"}},"save":{"g":"","p":{}},"stale":{"g":"","p":{}},"reg":{"g":"control_inline_2_01_16","p":{"has_inline_labels":"false"}},"reg_vp":{"g":"test_group_1","p":{"hide_value_prop":"true"}},"prof_pic_upsell":{"g":"","p":{}},"prof_pic_creation":{"g":"","p":{}},"onetaplogin":{"g":"","p":{}},"onetaplogin_userbased":{"g":"","p":{}},"feed_vp":{"g":"","p":{}},"push_notifications":{"g":"","p":{}},"login_poe":{"g":"","p":{}},"report_haf":{"g":"","p":{}},"report_profile":{"g":"","p":{}},"reporting":{"g":"","p":{}},"media_reporting":{"g":"","p":{}},"bg_sync":{"g":"","p":{}},"disc_ppl":{"g":"","p":{}},"ebdsim_li":{"g":"","p":{}},"ebdsim_lo":{"g":"","p":{}},"embeds":{"g":"","p":{}},"prvcy_tggl":{"g":"","p":{}},"tp_pblshr":{"g":"","p":{}},"fs":{"g":"","p":{}},"404_as_react":{"g":"","p":{}},"acc_recovery":{"g":"","p":{}},"connections":{"g":"","p":{}}},"hostname":"www.instagram.com","display_properties_server_guess":{"pixel_ratio":1.5,"viewport_width":360,"viewport_height":480,"orientation":""},"environment_switcher_visible_server_guess":true,"platform":"web","nonce":"k05odc1FHtEW7COQpskzNQ==","zero_data":{},"is_canary":true,"rollout_hash":"5382794631a5","probably_has_app":false,"show_app_install":true};
@@ -893,6 +893,58 @@
   </si>
   <si>
     <t>http://www.srdrylmz.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+window._sharedData = {"activity_counts":null,"config":{"csrf_token":"QGh4jEgw3mKVRnpPPUJgUvipRa5wpAom","viewer":null},"country_code":"DE","language_code":"en","locale":"en_US","entry_data":{"ProfilePage":[{"user":{"biography":"\u003c\u003c\u003c\u003cComputer Engineer\u003e\u003e\u003e\u003e\n     MPAL \u0026 SA\u00dc Graduated\n              Bursa \u2708\ufe0f Berlin\n                    Archer \n______________\ud83c\uddf9\ud83c\uddf7_____________","blocked_by_viewer":false,"country_block":false,"external_url":null,"external_url_linkshimmed":null,"followed_by":{"count":545},"followed_by_viewer":false,"follows":{"count":299},"follows_viewer":false,"full_name":"____________\u003cTK\u003e____________","has_blocked_viewer":false,"has_requested_viewer":false,"id":"1700499581","is_private":true,"is_verified":false,"mutual_followers":null,"profile_pic_url":"https://scontent-frx5-1.cdninstagram.com/vp/ae8cca32468cae276fd70a823898fcc1/5B28BE4A/t51.2885-19/s150x150/26866731_836251886546942_8991696596055883776_n.jpg","profile_pic_url_hd":"https://scontent-frx5-1.cdninstagram.com/vp/e53ac13652c0e170cd623c31c3e73385/5B18ABBA/t51.2885-19/s320x320/26866731_836251886546942_8991696596055883776_n.jpg","requested_by_viewer":false,"username":"tlgkyck","connected_fb_page":null,"media":{"nodes":[],"count":209,"page_info":{"has_next_page":true,"end_cursor":"AQAmcvNgNQdXrX-yWHJTeZehxjx_2bY_bzfGXy_ImMgrcSPJf06SGb8eTYQNBcB94hBQ9rANqyxHR22a4TdP_olRs5dtqun5jdHj0B5-eyQ-rA"}},"saved_media":{"nodes":[],"count":0,"page_info":{"has_next_page":false,"end_cursor":null}},"media_collections":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]}},"logging_page_id":"profilePage_1700499581","show_suggested_profiles":false,"graphql":{"user":{"biography":"\u003c\u003c\u003c\u003cComputer Engineer\u003e\u003e\u003e\u003e\n     MPAL \u0026 SA\u00dc Graduated\n              Bursa \u2708\ufe0f Berlin\n                    Archer \n______________\ud83c\uddf9\ud83c\uddf7_____________","blocked_by_viewer":false,"country_block":false,"external_url":null,"external_url_linkshimmed":null,"edge_followed_by":{"count":545},"followed_by_viewer":false,"edge_follow":{"count":299},"follows_viewer":false,"full_name":"____________\u003cTK\u003e____________","has_blocked_viewer":false,"has_requested_viewer":false,"id":"1700499581","is_private":true,"is_verified":false,"mutual_followers":null,"profile_pic_url":"https://scontent-frx5-1.cdninstagram.com/vp/ae8cca32468cae276fd70a823898fcc1/5B28BE4A/t51.2885-19/s150x150/26866731_836251886546942_8991696596055883776_n.jpg","profile_pic_url_hd":"https://scontent-frx5-1.cdninstagram.com/vp/e53ac13652c0e170cd623c31c3e73385/5B18ABBA/t51.2885-19/s320x320/26866731_836251886546942_8991696596055883776_n.jpg","requested_by_viewer":false,"username":"tlgkyck","connected_fb_page":null,"edge_owner_to_timeline_media":{"count":209,"page_info":{"has_next_page":true,"end_cursor":"AQAmcvNgNQdXrX-yWHJTeZehxjx_2bY_bzfGXy_ImMgrcSPJf06SGb8eTYQNBcB94hBQ9rANqyxHR22a4TdP_olRs5dtqun5jdHj0B5-eyQ-rA"},"edges":[]},"edge_saved_media":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]},"edge_media_collections":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]}}}}]},"gatekeepers":{"ld":true,"seo":true},"qe":{"834cfd9a":{"g":"","p":{}},"client_gql":{"g":"","p":{}},"b57bc793":{"g":"","p":{}},"dash_for_vod":{"g":"","p":{}},"f6b232bb":{"g":"","p":{}},"bc3l":{"g":"","p":{}},"a47f578c":{"g":"","p":{}},"aysf":{"g":"","p":{}},"04eaabb0":{"g":"","p":{}},"notif":{"g":"","p":{}},"25b356ab":{"g":"","p":{}},"follow_button":{"g":"","p":{}},"e2cffd31":{"g":"launch","p":{"new_cta":"true","remove_upsell_banner":"true","update_nav":"true"}},"loggedout":{"g":"launch","p":{"new_cta":"true","remove_upsell_banner":"true","update_nav":"true"}},"8a5c80fd":{"g":"","p":{}},"loggedout_upsell":{"g":"","p":{}},"bd6730a0":{"g":"","p":{}},"stories":{"g":"","p":{}},"76a86dfb":{"g":"","p":{}},"exit_story_creation":{"g":"","p":{}},"df78c718":{"g":"","p":{}},"su_universe":{"g":"","p":{}},"11bbbc09":{"g":"","p":{}},"us_li":{"g":"","p":{}},"d16c94c5":{"g":"","p":{}},"sidecar":{"g":"","p":{}},"af886adf":{"g":"","p":{}},"video":{"g":"","p":{}},"bb21ed8b":{"g":"","p":{}},"appsell":{"g":"","p":{}},"78e2146b":{"g":"","p":{}},"collections":{"g":"","p":{}},"47d6a3b3":{"g":"test_prefill_2_15","p":{"has_msisdn_prefill":"true"}},"msisdn":{"g":"test_prefill_2_15","p":{"has_msisdn_prefill":"true"}},"4ae576c1":{"g":"","p":{}},"save":{"g":"","p":{}},"9dcf4750":{"g":"","p":{}},"stale":{"g":"","p":{}},"edc7f6d2":{"g":"","p":{}},"reg":{"g":"","p":{}},"47ce4b24":{"g":"control_group_1","p":{"hide_value_prop":"false"}},"reg_vp":{"g":"control_group_1","p":{"hide_value_prop":"false"}},"1df00ebb":{"g":"","p":{}},"prof_pic_upsell":{"g":"","p":{}},"004e9939":{"g":"","p":{}},"prof_pic_creation":{"g":"","p":{}},"fbce4ce4":{"g":"","p":{}},"onetaplogin":{"g":"","p":{}},"b239bf2d":{"g":"","p":{}},"onetaplogin_userbased":{"g":"","p":{}},"6bf718a8":{"g":"","p":{}},"feed_vp":{"g":"","p":{}},"8365e413":{"g":"","p":{}},"push_notifications":{"g":"","p":{}},"94df4b40":{"g":"","p":{}},"login_poe":{"g":"","p":{}},"4844df36":{"g":"","p":{}},"report_haf":{"g":"","p":{}},"f4651ae9":{"g":"","p":{}},"report_profile":{"g":"","p":{}},"47d2aebf":{"g":"","p":{}},"reporting":{"g":"","p":{}},"cb1ff25c":{"g":"","p":{}},"media_reporting":{"g":"","p":{}},"0d3bf783":{"g":"","p":{}},"bg_sync":{"g":"","p":{}},"ea55ef64":{"g":"","p":{}},"disc_ppl":{"g":"","p":{}},"28cc279b":{"g":"","p":{}},"ebdsim_li":{"g":"","p":{}},"3c0bc5c7":{"g":"","p":{}},"ebdsim_lo":{"g":"","p":{}},"d5dde92a":{"g":"","p":{}},"embeds":{"g":"","p":{}},"ca7fa6dd":{"g":"","p":{}},"prvcy_tggl":{"g":"","p":{}},"608b2c6c":{"g":"","p":{}},"tp_pblshr":{"g":"","p":{}},"2ea1c751":{"g":"","p":{}},"fs":{"g":"","p":{}},"b212f68e":{"g":"","p":{}},"404_as_react":{"g":"","p":{}},"d8c67ea6":{"g":"","p":{}},"acc_recovery":{"g":"","p":{}},"e878cb91":{"g":"","p":{}},"connections":{"g":"","p":{}}},"hostname":"www.instagram.com","display_properties_server_guess":{"pixel_ratio":1.5,"viewport_width":360,"viewport_height":480,"orientation":""},"environment_switcher_visible_server_guess":true,"platform":"web","nonce":"nhuYXH4EZG7A3DVB66+4iA==","zero_data":{},"rollout_hash":"3156f3856bb5","probably_has_app":false,"show_app_install":true};
+!function(e){function a(n){if(o[n])return o[n].exports;var t=o[n]={i:n,l:!1,exports:{}};return e[n].call(t.exports,t,t.exports,a),t.l=!0,t.exports}var n=window.webpackJsonp;window.webpackJsonp=function(o,r,i){for(var c,d,s,g=0,f=[];g&lt;o.length;g++)d=o[g],t[d]&amp;&amp;f.push(t[d][0]),t[d]=0;for(c in r)Object.prototype.hasOwnProperty.call(r,c)&amp;&amp;(e[c]=r[c]);for(n&amp;&amp;n(o,r,i);f.length;)f.shift()();if(i)for(g=0;g&lt;i.length;g++)s=a(a.s=i[g]);return s};var o={},t={49:0};a.e=function(e){function n(){c.onerror=c.onload=null,clearTimeout(d);var a=t[e];0!==a&amp;&amp;(a&amp;&amp;a[1](new Error("Loading chunk "+e+" failed.")),t[e]=void 0)}var o=t[e];if(0===o)return new Promise(function(e){e()});if(o)return o[2];var r=new Promise(function(a,n){o=t[e]=[a,n]});o[2]=r;var i=document.getElementsByTagName("head")[0],c=document.createElement("script");c.type="text/javascript",c.charset="utf-8",c.async=!0,c.timeout=12e4,c.crossOrigin="anonymous",a.nc&amp;&amp;c.setAttribute("nonce",a.nc),c.src=a.p+""+({0:"SettingsModules",1:"ProfilePageContainer",2:"LikedByListContainer",3:"FollowListContainer",4:"CreationModules",5:"LocationPageContainer",6:"DiscoverMediaPageContainer",7:"DiscoverEmbedsPageContainer",8:"UserCollectionMediaPageContainer",9:"TagPageContainer",10:"DebugInfoNub",11:"FeedPageContainer",12:"LandingPage",13:"PostPageContainer",14:"LoginAndSignupPage",15:"ResetPasswordPageContainer",16:"UserCollectionsPageContainer",17:"MobileStoriesPage",18:"DesktopStoriesPage",19:"DiscoverPeoplePageContainer",20:"MultiStepSignupPage",21:"ContactHistoryPage",22:"LocationsDirectoryLandingPage",23:"LocationsDirectoryCountryPage",24:"LocationsDirectoryCityPage",25:"EmailConfirmationPage",26:"SuggestedDirectoryLandingPage",27:"ProfilesDirectoryLandingPage",28:"DirectoryPage",29:"HttpErrorPage",30:"ActivityFeedPage",31:"CameraPage",32:"StoryCreationPage",33:"NewUserInterstitial",34:"FBSignupPage",35:"ContactInvitesOptOutPage",36:"Report",37:"Copyright",38:"SupportInfo",39:"Community",40:"GenericSurvey",41:"Challenge",42:"Consumer",43:"EmailSnoozePage",44:"EmailUnsubscribePage",45:"ConfirmFollowDialog",46:"NotificationLandingPage"}[e]||e)+".js/"+{0:"34ea21d19385",1:"88a1a465402e",2:"2342482c75ef",3:"b9dcacbeebc8",4:"c1984d97bc70",5:"288026a6de18",6:"109f6d734863",7:"9e82b7c6ea0b",8:"c9e9bb9efe11",9:"92c450f75f4b",10:"1197ccc46117",11:"3dfd8fa6cfd8",12:"12285bb0b069",13:"27c91aa59fdd",14:"d0a40e755e1e",15:"dd787adc92eb",16:"a4a16427cde3",17:"5800bb273aaa",18:"0703aab3b464",19:"90a8b57ae564",20:"41fa98f6895a",21:"5e044281585c",22:"6858feeb0a66",23:"d1c754295774",24:"7ea767ae76ee",25:"923742376262",26:"d5d5986f3842",27:"1352aea86cc0",28:"bd34aef749f3",29:"762c22ea65a3",30:"d366074da593",31:"ac0ef7598973",32:"fec058817877",33:"e037bebe8036",34:"6c4311554b3b",35:"95a47539d8b2",36:"494c93e40323",37:"5f29e1fddd91",38:"d9582b7fd06a",39:"3c182b8237da",40:"66ae1b2c8d3e",41:"ff6fd0e21ca6",42:"3034c2271934",43:"ba7e7b31317a",44:"a77601a12715",45:"b4a125eea937",46:"30463ebe552b"}[e]+".js";var d=setTimeout(n,12e4);return c.onerror=c.onload=n,i.appendChild(c),r},a.m=e,a.c=o,a.d=function(e,n,o){a.o(e,n)||Object.defineProperty(e,n,{configurable:!1,enumerable:!0,get:o})},a.n=function(e){var n=e&amp;&amp;e.__esModule?function(){return e.default}:function(){return e};return a.d(n,"a",n),n},a.o=function(e,a){return Object.prototype.hasOwnProperty.call(e,a)},a.p="/static/bundles/",a.oe=function(e){throw console.error(e),e}}([]);
+!function(f,b,e,v,n,t,s){if(f.fbq)return;n=f.fbq=function(){n.callMethod?
+n.callMethod.apply(n,arguments):n.queue.push(arguments)};if(!f._fbq)f._fbq=n;
+n.push=n;n.loaded=!0;n.version='2.0';n.queue=[];t=b.createElement(e);t.async=!0;
+t.src=v;s=b.getElementsByTagName(e)[0];s.parentNode.insertBefore(t,s)}(window,
+document,'script','//connect.facebook.net/en_US/fbevents.js');
+fbq('init', '1425767024389221');
+fbq('track', 'PageView');
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+window._sharedData = {"activity_counts":null,"config":{"csrf_token":"RkJe3RQ5hN0ZRYfZQvLCuo3hJs3DgtBj","viewer":null},"country_code":"DE","language_code":"en","locale":"en_US","entry_data":{"ProfilePage":[{"user":{"biography":"\u003c\u003c\u003c\u003cComputer Engineer\u003e\u003e\u003e\u003e\n     MPAL \u0026 SA\u00dc Graduated\n              Bursa \u2708\ufe0f Berlin\n                    Archer \n______________\ud83c\uddf9\ud83c\uddf7_____________","blocked_by_viewer":false,"country_block":false,"external_url":null,"external_url_linkshimmed":null,"followed_by":{"count":545},"followed_by_viewer":false,"follows":{"count":299},"follows_viewer":false,"full_name":"____________\u003cTK\u003e____________","has_blocked_viewer":false,"has_requested_viewer":false,"id":"1700499581","is_private":true,"is_verified":false,"mutual_followers":null,"profile_pic_url":"https://scontent-frx5-1.cdninstagram.com/vp/ae8cca32468cae276fd70a823898fcc1/5B28BE4A/t51.2885-19/s150x150/26866731_836251886546942_8991696596055883776_n.jpg","profile_pic_url_hd":"https://scontent-frx5-1.cdninstagram.com/vp/e53ac13652c0e170cd623c31c3e73385/5B18ABBA/t51.2885-19/s320x320/26866731_836251886546942_8991696596055883776_n.jpg","requested_by_viewer":false,"username":"tlgkyck","connected_fb_page":null,"media":{"nodes":[],"count":209,"page_info":{"has_next_page":true,"end_cursor":"AQB-iZdIyT51bGb5fUXf78xE6PPZmPqvVYEnuQGhy8Gmx1TpLJUISBuGf366OIOrOtEYsa2z0_xoe22IiTCO35xp_UB1iCjcBMSPKa-JzeUM5Q"}},"saved_media":{"nodes":[],"count":0,"page_info":{"has_next_page":false,"end_cursor":null}},"media_collections":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]}},"logging_page_id":"profilePage_1700499581","show_suggested_profiles":false,"graphql":{"user":{"biography":"\u003c\u003c\u003c\u003cComputer Engineer\u003e\u003e\u003e\u003e\n     MPAL \u0026 SA\u00dc Graduated\n              Bursa \u2708\ufe0f Berlin\n                    Archer \n______________\ud83c\uddf9\ud83c\uddf7_____________","blocked_by_viewer":false,"country_block":false,"external_url":null,"external_url_linkshimmed":null,"edge_followed_by":{"count":545},"followed_by_viewer":false,"edge_follow":{"count":299},"follows_viewer":false,"full_name":"____________\u003cTK\u003e____________","has_blocked_viewer":false,"has_requested_viewer":false,"id":"1700499581","is_private":true,"is_verified":false,"mutual_followers":null,"profile_pic_url":"https://scontent-frx5-1.cdninstagram.com/vp/ae8cca32468cae276fd70a823898fcc1/5B28BE4A/t51.2885-19/s150x150/26866731_836251886546942_8991696596055883776_n.jpg","profile_pic_url_hd":"https://scontent-frx5-1.cdninstagram.com/vp/e53ac13652c0e170cd623c31c3e73385/5B18ABBA/t51.2885-19/s320x320/26866731_836251886546942_8991696596055883776_n.jpg","requested_by_viewer":false,"username":"tlgkyck","connected_fb_page":null,"edge_owner_to_timeline_media":{"count":209,"page_info":{"has_next_page":true,"end_cursor":"AQB-iZdIyT51bGb5fUXf78xE6PPZmPqvVYEnuQGhy8Gmx1TpLJUISBuGf366OIOrOtEYsa2z0_xoe22IiTCO35xp_UB1iCjcBMSPKa-JzeUM5Q"},"edges":[]},"edge_saved_media":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]},"edge_media_collections":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]}}}}]},"gatekeepers":{"ld":true,"seo":true},"qe":{"834cfd9a":{"g":"","p":{}},"client_gql":{"g":"","p":{}},"b57bc793":{"g":"","p":{}},"dash_for_vod":{"g":"","p":{}},"f6b232bb":{"g":"","p":{}},"bc3l":{"g":"","p":{}},"a47f578c":{"g":"","p":{}},"aysf":{"g":"","p":{}},"04eaabb0":{"g":"","p":{}},"notif":{"g":"","p":{}},"25b356ab":{"g":"","p":{}},"follow_button":{"g":"","p":{}},"e2cffd31":{"g":"launch","p":{"new_cta":"true","remove_upsell_banner":"true","update_nav":"true"}},"loggedout":{"g":"launch","p":{"new_cta":"true","remove_upsell_banner":"true","update_nav":"true"}},"8a5c80fd":{"g":"","p":{}},"loggedout_upsell":{"g":"","p":{}},"bd6730a0":{"g":"","p":{}},"stories":{"g":"","p":{}},"76a86dfb":{"g":"","p":{}},"exit_story_creation":{"g":"","p":{}},"df78c718":{"g":"","p":{}},"su_universe":{"g":"","p":{}},"11bbbc09":{"g":"","p":{}},"us_li":{"g":"","p":{}},"d16c94c5":{"g":"","p":{}},"sidecar":{"g":"","p":{}},"af886adf":{"g":"","p":{}},"video":{"g":"","p":{}},"bb21ed8b":{"g":"","p":{}},"appsell":{"g":"","p":{}},"78e2146b":{"g":"","p":{}},"collections":{"g":"","p":{}},"47d6a3b3":{"g":"control_prefill_2_15","p":{"has_msisdn_prefill":"false"}},"msisdn":{"g":"control_prefill_2_15","p":{"has_msisdn_prefill":"false"}},"4ae576c1":{"g":"","p":{}},"save":{"g":"","p":{}},"9dcf4750":{"g":"","p":{}},"stale":{"g":"","p":{}},"edc7f6d2":{"g":"new_reg_with_appsells_01_10","p":{"has_new_landing_appsells":"true","has_new_landing_page":"true"}},"reg":{"g":"new_reg_with_appsells_01_10","p":{"has_new_landing_appsells":"true","has_new_landing_page":"true"}},"47ce4b24":{"g":"control_group_1","p":{"hide_value_prop":"false"}},"reg_vp":{"g":"control_group_1","p":{"hide_value_prop":"false"}},"1df00ebb":{"g":"","p":{}},"prof_pic_upsell":{"g":"","p":{}},"004e9939":{"g":"","p":{}},"prof_pic_creation":{"g":"","p":{}},"fbce4ce4":{"g":"","p":{}},"onetaplogin":{"g":"","p":{}},"b239bf2d":{"g":"","p":{}},"onetaplogin_userbased":{"g":"","p":{}},"6bf718a8":{"g":"","p":{}},"feed_vp":{"g":"","p":{}},"8365e413":{"g":"","p":{}},"push_notifications":{"g":"","p":{}},"94df4b40":{"g":"","p":{}},"login_poe":{"g":"","p":{}},"4844df36":{"g":"","p":{}},"report_haf":{"g":"","p":{}},"f4651ae9":{"g":"","p":{}},"report_profile":{"g":"","p":{}},"47d2aebf":{"g":"","p":{}},"reporting":{"g":"","p":{}},"cb1ff25c":{"g":"","p":{}},"media_reporting":{"g":"","p":{}},"0d3bf783":{"g":"","p":{}},"bg_sync":{"g":"","p":{}},"ea55ef64":{"g":"","p":{}},"disc_ppl":{"g":"","p":{}},"28cc279b":{"g":"","p":{}},"ebdsim_li":{"g":"","p":{}},"3c0bc5c7":{"g":"","p":{}},"ebdsim_lo":{"g":"","p":{}},"d5dde92a":{"g":"","p":{}},"embeds":{"g":"","p":{}},"ca7fa6dd":{"g":"","p":{}},"prvcy_tggl":{"g":"","p":{}},"608b2c6c":{"g":"","p":{}},"tp_pblshr":{"g":"","p":{}},"2ea1c751":{"g":"","p":{}},"fs":{"g":"","p":{}},"b212f68e":{"g":"","p":{}},"404_as_react":{"g":"","p":{}},"d8c67ea6":{"g":"","p":{}},"acc_recovery":{"g":"","p":{}},"e878cb91":{"g":"","p":{}},"connections":{"g":"","p":{}}},"hostname":"www.instagram.com","display_properties_server_guess":{"pixel_ratio":1.5,"viewport_width":360,"viewport_height":480,"orientation":""},"environment_switcher_visible_server_guess":true,"platform":"web","nonce":"NE+qMqVAxdlbi+xNYhAMCw==","zero_data":{},"rollout_hash":"3156f3856bb5","probably_has_app":false,"show_app_install":true};
+!function(e){function a(n){if(o[n])return o[n].exports;var t=o[n]={i:n,l:!1,exports:{}};return e[n].call(t.exports,t,t.exports,a),t.l=!0,t.exports}var n=window.webpackJsonp;window.webpackJsonp=function(o,r,i){for(var c,d,s,g=0,f=[];g&lt;o.length;g++)d=o[g],t[d]&amp;&amp;f.push(t[d][0]),t[d]=0;for(c in r)Object.prototype.hasOwnProperty.call(r,c)&amp;&amp;(e[c]=r[c]);for(n&amp;&amp;n(o,r,i);f.length;)f.shift()();if(i)for(g=0;g&lt;i.length;g++)s=a(a.s=i[g]);return s};var o={},t={49:0};a.e=function(e){function n(){c.onerror=c.onload=null,clearTimeout(d);var a=t[e];0!==a&amp;&amp;(a&amp;&amp;a[1](new Error("Loading chunk "+e+" failed.")),t[e]=void 0)}var o=t[e];if(0===o)return new Promise(function(e){e()});if(o)return o[2];var r=new Promise(function(a,n){o=t[e]=[a,n]});o[2]=r;var i=document.getElementsByTagName("head")[0],c=document.createElement("script");c.type="text/javascript",c.charset="utf-8",c.async=!0,c.timeout=12e4,c.crossOrigin="anonymous",a.nc&amp;&amp;c.setAttribute("nonce",a.nc),c.src=a.p+""+({0:"SettingsModules",1:"ProfilePageContainer",2:"LikedByListContainer",3:"FollowListContainer",4:"CreationModules",5:"LocationPageContainer",6:"DiscoverMediaPageContainer",7:"DiscoverEmbedsPageContainer",8:"UserCollectionMediaPageContainer",9:"TagPageContainer",10:"DebugInfoNub",11:"FeedPageContainer",12:"LandingPage",13:"PostPageContainer",14:"LoginAndSignupPage",15:"ResetPasswordPageContainer",16:"UserCollectionsPageContainer",17:"MobileStoriesPage",18:"DesktopStoriesPage",19:"DiscoverPeoplePageContainer",20:"MultiStepSignupPage",21:"ContactHistoryPage",22:"LocationsDirectoryLandingPage",23:"LocationsDirectoryCountryPage",24:"LocationsDirectoryCityPage",25:"EmailConfirmationPage",26:"SuggestedDirectoryLandingPage",27:"ProfilesDirectoryLandingPage",28:"DirectoryPage",29:"HttpErrorPage",30:"ActivityFeedPage",31:"CameraPage",32:"StoryCreationPage",33:"NewUserInterstitial",34:"FBSignupPage",35:"ContactInvitesOptOutPage",36:"Report",37:"Copyright",38:"SupportInfo",39:"Community",40:"GenericSurvey",41:"Challenge",42:"Consumer",43:"EmailSnoozePage",44:"EmailUnsubscribePage",45:"ConfirmFollowDialog",46:"NotificationLandingPage"}[e]||e)+".js/"+{0:"34ea21d19385",1:"88a1a465402e",2:"2342482c75ef",3:"b9dcacbeebc8",4:"c1984d97bc70",5:"288026a6de18",6:"109f6d734863",7:"9e82b7c6ea0b",8:"c9e9bb9efe11",9:"92c450f75f4b",10:"1197ccc46117",11:"3dfd8fa6cfd8",12:"12285bb0b069",13:"27c91aa59fdd",14:"d0a40e755e1e",15:"dd787adc92eb",16:"a4a16427cde3",17:"5800bb273aaa",18:"0703aab3b464",19:"90a8b57ae564",20:"41fa98f6895a",21:"5e044281585c",22:"6858feeb0a66",23:"d1c754295774",24:"7ea767ae76ee",25:"923742376262",26:"d5d5986f3842",27:"1352aea86cc0",28:"bd34aef749f3",29:"762c22ea65a3",30:"d366074da593",31:"ac0ef7598973",32:"fec058817877",33:"e037bebe8036",34:"6c4311554b3b",35:"95a47539d8b2",36:"494c93e40323",37:"5f29e1fddd91",38:"d9582b7fd06a",39:"3c182b8237da",40:"66ae1b2c8d3e",41:"ff6fd0e21ca6",42:"3034c2271934",43:"ba7e7b31317a",44:"a77601a12715",45:"b4a125eea937",46:"30463ebe552b"}[e]+".js";var d=setTimeout(n,12e4);return c.onerror=c.onload=n,i.appendChild(c),r},a.m=e,a.c=o,a.d=function(e,n,o){a.o(e,n)||Object.defineProperty(e,n,{configurable:!1,enumerable:!0,get:o})},a.n=function(e){var n=e&amp;&amp;e.__esModule?function(){return e.default}:function(){return e};return a.d(n,"a",n),n},a.o=function(e,a){return Object.prototype.hasOwnProperty.call(e,a)},a.p="/static/bundles/",a.oe=function(e){throw console.error(e),e}}([]);
+!function(f,b,e,v,n,t,s){if(f.fbq)return;n=f.fbq=function(){n.callMethod?
+n.callMethod.apply(n,arguments):n.queue.push(arguments)};if(!f._fbq)f._fbq=n;
+n.push=n;n.loaded=!0;n.version='2.0';n.queue=[];t=b.createElement(e);t.async=!0;
+t.src=v;s=b.getElementsByTagName(e)[0];s.parentNode.insertBefore(t,s)}(window,
+document,'script','//connect.facebook.net/en_US/fbevents.js');
+fbq('init', '1425767024389221');
+fbq('track', 'PageView');
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+window._sharedData = {"activity_counts":null,"config":{"csrf_token":"AayIhlcxLxmekeLljc9riQwbyKrqS5Sc","viewer":null},"country_code":"DE","language_code":"en","locale":"en_US","entry_data":{"ProfilePage":[{"user":{"biography":"\u003c\u003c\u003c\u003cComputer Engineer\u003e\u003e\u003e\u003e\n     MPAL \u0026 SA\u00dc Graduated\n              Bursa \u2708\ufe0f Berlin\n                    Archer \n______________\ud83c\uddf9\ud83c\uddf7_____________","blocked_by_viewer":false,"country_block":false,"external_url":null,"external_url_linkshimmed":null,"followed_by":{"count":547},"followed_by_viewer":false,"follows":{"count":299},"follows_viewer":false,"full_name":"____________\u003cTK\u003e____________","has_blocked_viewer":false,"has_requested_viewer":false,"id":"1700499581","is_private":true,"is_verified":false,"mutual_followers":null,"profile_pic_url":"https://scontent-frx5-1.cdninstagram.com/vp/ae8cca32468cae276fd70a823898fcc1/5B28BE4A/t51.2885-19/s150x150/26866731_836251886546942_8991696596055883776_n.jpg","profile_pic_url_hd":"https://scontent-frx5-1.cdninstagram.com/vp/e53ac13652c0e170cd623c31c3e73385/5B18ABBA/t51.2885-19/s320x320/26866731_836251886546942_8991696596055883776_n.jpg","requested_by_viewer":false,"username":"tlgkyck","connected_fb_page":null,"media":{"nodes":[],"count":209,"page_info":{"has_next_page":true,"end_cursor":"AQCKUAYH0Y-YVKG7qkdKkZli1t29Pk_ArpM8O7XkeYq7GguPUCNvwOW9m4kshsgSTeCQXrdOyCKZTrXbtiypKrAERrasNJ6jEB1OWx8fLQe45A"}},"saved_media":{"nodes":[],"count":0,"page_info":{"has_next_page":false,"end_cursor":null}},"media_collections":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]}},"logging_page_id":"profilePage_1700499581","show_suggested_profiles":false,"graphql":{"user":{"biography":"\u003c\u003c\u003c\u003cComputer Engineer\u003e\u003e\u003e\u003e\n     MPAL \u0026 SA\u00dc Graduated\n              Bursa \u2708\ufe0f Berlin\n                    Archer \n______________\ud83c\uddf9\ud83c\uddf7_____________","blocked_by_viewer":false,"country_block":false,"external_url":null,"external_url_linkshimmed":null,"edge_followed_by":{"count":547},"followed_by_viewer":false,"edge_follow":{"count":299},"follows_viewer":false,"full_name":"____________\u003cTK\u003e____________","has_blocked_viewer":false,"has_requested_viewer":false,"id":"1700499581","is_private":true,"is_verified":false,"mutual_followers":null,"profile_pic_url":"https://scontent-frx5-1.cdninstagram.com/vp/ae8cca32468cae276fd70a823898fcc1/5B28BE4A/t51.2885-19/s150x150/26866731_836251886546942_8991696596055883776_n.jpg","profile_pic_url_hd":"https://scontent-frx5-1.cdninstagram.com/vp/e53ac13652c0e170cd623c31c3e73385/5B18ABBA/t51.2885-19/s320x320/26866731_836251886546942_8991696596055883776_n.jpg","requested_by_viewer":false,"username":"tlgkyck","connected_fb_page":null,"edge_owner_to_timeline_media":{"count":209,"page_info":{"has_next_page":true,"end_cursor":"AQCKUAYH0Y-YVKG7qkdKkZli1t29Pk_ArpM8O7XkeYq7GguPUCNvwOW9m4kshsgSTeCQXrdOyCKZTrXbtiypKrAERrasNJ6jEB1OWx8fLQe45A"},"edges":[]},"edge_saved_media":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]},"edge_media_collections":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]}}}}]},"gatekeepers":{"ld":true,"seo":true},"qe":{"834cfd9a":{"g":"","p":{}},"client_gql":{"g":"","p":{}},"b57bc793":{"g":"","p":{}},"dash_for_vod":{"g":"","p":{}},"f6b232bb":{"g":"","p":{}},"bc3l":{"g":"","p":{}},"a47f578c":{"g":"","p":{}},"aysf":{"g":"","p":{}},"04eaabb0":{"g":"","p":{}},"notif":{"g":"","p":{}},"25b356ab":{"g":"","p":{}},"follow_button":{"g":"","p":{}},"e2cffd31":{"g":"launch","p":{"new_cta":"true","remove_upsell_banner":"true","update_nav":"true"}},"loggedout":{"g":"launch","p":{"new_cta":"true","remove_upsell_banner":"true","update_nav":"true"}},"8a5c80fd":{"g":"","p":{}},"loggedout_upsell":{"g":"","p":{}},"bd6730a0":{"g":"","p":{}},"stories":{"g":"","p":{}},"76a86dfb":{"g":"","p":{}},"exit_story_creation":{"g":"","p":{}},"df78c718":{"g":"test_msisdn_prefill_12_18","p":{"has_msisdn_prefill":"true"}},"su_universe":{"g":"test_msisdn_prefill_12_18","p":{"has_msisdn_prefill":"true"}},"11bbbc09":{"g":"","p":{}},"us_li":{"g":"","p":{}},"d16c94c5":{"g":"","p":{}},"sidecar":{"g":"","p":{}},"af886adf":{"g":"","p":{}},"video":{"g":"","p":{}},"bb21ed8b":{"g":"","p":{}},"appsell":{"g":"","p":{}},"78e2146b":{"g":"","p":{}},"collections":{"g":"","p":{}},"47d6a3b3":{"g":"test_prefill_2_15","p":{"has_msisdn_prefill":"true"}},"msisdn":{"g":"test_prefill_2_15","p":{"has_msisdn_prefill":"true"}},"4ae576c1":{"g":"","p":{}},"save":{"g":"","p":{}},"9dcf4750":{"g":"","p":{}},"stale":{"g":"","p":{}},"edc7f6d2":{"g":"","p":{}},"reg":{"g":"","p":{}},"47ce4b24":{"g":"","p":{}},"reg_vp":{"g":"","p":{}},"1df00ebb":{"g":"","p":{}},"prof_pic_upsell":{"g":"","p":{}},"004e9939":{"g":"","p":{}},"prof_pic_creation":{"g":"","p":{}},"fbce4ce4":{"g":"","p":{}},"onetaplogin":{"g":"","p":{}},"b239bf2d":{"g":"","p":{}},"onetaplogin_userbased":{"g":"","p":{}},"6bf718a8":{"g":"","p":{}},"feed_vp":{"g":"","p":{}},"8365e413":{"g":"","p":{}},"push_notifications":{"g":"","p":{}},"94df4b40":{"g":"","p":{}},"login_poe":{"g":"","p":{}},"4844df36":{"g":"","p":{}},"report_haf":{"g":"","p":{}},"f4651ae9":{"g":"","p":{}},"report_profile":{"g":"","p":{}},"47d2aebf":{"g":"","p":{}},"reporting":{"g":"","p":{}},"cb1ff25c":{"g":"","p":{}},"media_reporting":{"g":"","p":{}},"0d3bf783":{"g":"","p":{}},"bg_sync":{"g":"","p":{}},"ea55ef64":{"g":"","p":{}},"disc_ppl":{"g":"","p":{}},"28cc279b":{"g":"","p":{}},"ebdsim_li":{"g":"","p":{}},"3c0bc5c7":{"g":"","p":{}},"ebdsim_lo":{"g":"","p":{}},"d5dde92a":{"g":"","p":{}},"embeds":{"g":"","p":{}},"ca7fa6dd":{"g":"","p":{}},"prvcy_tggl":{"g":"","p":{}},"608b2c6c":{"g":"","p":{}},"tp_pblshr":{"g":"","p":{}},"2ea1c751":{"g":"","p":{}},"fs":{"g":"","p":{}},"b212f68e":{"g":"","p":{}},"404_as_react":{"g":"","p":{}},"d8c67ea6":{"g":"","p":{}},"acc_recovery":{"g":"","p":{}},"e878cb91":{"g":"","p":{}},"connections":{"g":"","p":{}},"0370381b":{"g":"","p":{}},"notif_banner":{"g":"","p":{}},"3b5f1021":{"g":"","p":{}},"private_lo":{"g":"","p":{}}},"hostname":"www.instagram.com","display_properties_server_guess":{"pixel_ratio":1.5,"viewport_width":360,"viewport_height":480,"orientation":""},"environment_switcher_visible_server_guess":true,"platform":"web","nonce":"u+RSpoKbgX2Vk7bq4Ww0Vw==","zero_data":{},"rollout_hash":"3156f3856bb5","probably_has_app":false,"show_app_install":true};
+!function(e){function a(n){if(o[n])return o[n].exports;var t=o[n]={i:n,l:!1,exports:{}};return e[n].call(t.exports,t,t.exports,a),t.l=!0,t.exports}var n=window.webpackJsonp;window.webpackJsonp=function(o,r,i){for(var c,d,s,g=0,f=[];g&lt;o.length;g++)d=o[g],t[d]&amp;&amp;f.push(t[d][0]),t[d]=0;for(c in r)Object.prototype.hasOwnProperty.call(r,c)&amp;&amp;(e[c]=r[c]);for(n&amp;&amp;n(o,r,i);f.length;)f.shift()();if(i)for(g=0;g&lt;i.length;g++)s=a(a.s=i[g]);return s};var o={},t={49:0};a.e=function(e){function n(){c.onerror=c.onload=null,clearTimeout(d);var a=t[e];0!==a&amp;&amp;(a&amp;&amp;a[1](new Error("Loading chunk "+e+" failed.")),t[e]=void 0)}var o=t[e];if(0===o)return new Promise(function(e){e()});if(o)return o[2];var r=new Promise(function(a,n){o=t[e]=[a,n]});o[2]=r;var i=document.getElementsByTagName("head")[0],c=document.createElement("script");c.type="text/javascript",c.charset="utf-8",c.async=!0,c.timeout=12e4,c.crossOrigin="anonymous",a.nc&amp;&amp;c.setAttribute("nonce",a.nc),c.src=a.p+""+({0:"SettingsModules",1:"ProfilePageContainer",2:"LikedByListContainer",3:"FollowListContainer",4:"CreationModules",5:"LocationPageContainer",6:"DiscoverMediaPageContainer",7:"DiscoverEmbedsPageContainer",8:"UserCollectionMediaPageContainer",9:"TagPageContainer",10:"DebugInfoNub",11:"FeedPageContainer",12:"LandingPage",13:"PostPageContainer",14:"LoginAndSignupPage",15:"ResetPasswordPageContainer",16:"UserCollectionsPageContainer",17:"MobileStoriesPage",18:"DesktopStoriesPage",19:"DiscoverPeoplePageContainer",20:"MultiStepSignupPage",21:"ContactHistoryPage",22:"LocationsDirectoryLandingPage",23:"LocationsDirectoryCountryPage",24:"LocationsDirectoryCityPage",25:"EmailConfirmationPage",26:"SuggestedDirectoryLandingPage",27:"ProfilesDirectoryLandingPage",28:"DirectoryPage",29:"HttpErrorPage",30:"ActivityFeedPage",31:"CameraPage",32:"StoryCreationPage",33:"NewUserInterstitial",34:"FBSignupPage",35:"ContactInvitesOptOutPage",36:"Report",37:"Copyright",38:"SupportInfo",39:"Community",40:"GenericSurvey",41:"Challenge",42:"Consumer",43:"EmailSnoozePage",44:"EmailUnsubscribePage",45:"ConfirmFollowDialog",46:"NotificationLandingPage"}[e]||e)+".js/"+{0:"34ea21d19385",1:"88a1a465402e",2:"2342482c75ef",3:"b9dcacbeebc8",4:"c1984d97bc70",5:"288026a6de18",6:"109f6d734863",7:"9e82b7c6ea0b",8:"c9e9bb9efe11",9:"92c450f75f4b",10:"1197ccc46117",11:"3dfd8fa6cfd8",12:"12285bb0b069",13:"27c91aa59fdd",14:"d0a40e755e1e",15:"dd787adc92eb",16:"a4a16427cde3",17:"5800bb273aaa",18:"0703aab3b464",19:"90a8b57ae564",20:"41fa98f6895a",21:"5e044281585c",22:"6858feeb0a66",23:"d1c754295774",24:"7ea767ae76ee",25:"923742376262",26:"d5d5986f3842",27:"1352aea86cc0",28:"bd34aef749f3",29:"762c22ea65a3",30:"d366074da593",31:"ac0ef7598973",32:"fec058817877",33:"e037bebe8036",34:"6c4311554b3b",35:"95a47539d8b2",36:"494c93e40323",37:"5f29e1fddd91",38:"d9582b7fd06a",39:"3c182b8237da",40:"66ae1b2c8d3e",41:"ff6fd0e21ca6",42:"3034c2271934",43:"ba7e7b31317a",44:"a77601a12715",45:"b4a125eea937",46:"30463ebe552b"}[e]+".js";var d=setTimeout(n,12e4);return c.onerror=c.onload=n,i.appendChild(c),r},a.m=e,a.c=o,a.d=function(e,n,o){a.o(e,n)||Object.defineProperty(e,n,{configurable:!1,enumerable:!0,get:o})},a.n=function(e){var n=e&amp;&amp;e.__esModule?function(){return e.default}:function(){return e};return a.d(n,"a",n),n},a.o=function(e,a){return Object.prototype.hasOwnProperty.call(e,a)},a.p="/static/bundles/",a.oe=function(e){throw console.error(e),e}}([]);
+!function(f,b,e,v,n,t,s){if(f.fbq)return;n=f.fbq=function(){n.callMethod?
+n.callMethod.apply(n,arguments):n.queue.push(arguments)};if(!f._fbq)f._fbq=n;
+n.push=n;n.loaded=!0;n.version='2.0';n.queue=[];t=b.createElement(e);t.async=!0;
+t.src=v;s=b.getElementsByTagName(e)[0];s.parentNode.insertBefore(t,s)}(window,
+document,'script','//connect.facebook.net/en_US/fbevents.js');
+fbq('init', '1425767024389221');
+fbq('track', 'PageView');
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+window._sharedData = {"activity_counts":null,"config":{"csrf_token":"WOB16fcTx3YgQM2IrzceKkTwCfzFeMr1","viewer":null},"country_code":"DE","language_code":"en","locale":"en_US","entry_data":{"ProfilePage":[{"user":{"biography":"\u003c\u003c\u003c\u003cComputer Engineer\u003e\u003e\u003e\u003e\n     MPAL \u0026 SA\u00dc Graduated\n              Bursa \u2708\ufe0f Berlin\n                    Archer \n______________\ud83c\uddf9\ud83c\uddf7_____________","blocked_by_viewer":false,"country_block":false,"external_url":null,"external_url_linkshimmed":null,"followed_by":{"count":547},"followed_by_viewer":false,"follows":{"count":299},"follows_viewer":false,"full_name":"____________\u003cTK\u003e____________","has_blocked_viewer":false,"has_requested_viewer":false,"id":"1700499581","is_private":true,"is_verified":false,"mutual_followers":null,"profile_pic_url":"https://scontent-frx5-1.cdninstagram.com/vp/ae8cca32468cae276fd70a823898fcc1/5B28BE4A/t51.2885-19/s150x150/26866731_836251886546942_8991696596055883776_n.jpg","profile_pic_url_hd":"https://scontent-frx5-1.cdninstagram.com/vp/e53ac13652c0e170cd623c31c3e73385/5B18ABBA/t51.2885-19/s320x320/26866731_836251886546942_8991696596055883776_n.jpg","requested_by_viewer":false,"username":"tlgkyck","connected_fb_page":null,"media":{"nodes":[],"count":209,"page_info":{"has_next_page":true,"end_cursor":"AQBpSHsXYn5mziP8mUv7z1JpUTbTwVNpTaqwngX03qrhG0LFkcmgQzDd9XQZ83SZZ7VWJs3UYQbYzjJzg6pQcnpS6J9KCbtoAaee8jYyHwyrkA"}},"saved_media":{"nodes":[],"count":0,"page_info":{"has_next_page":false,"end_cursor":null}},"media_collections":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]}},"logging_page_id":"profilePage_1700499581","show_suggested_profiles":false,"graphql":{"user":{"biography":"\u003c\u003c\u003c\u003cComputer Engineer\u003e\u003e\u003e\u003e\n     MPAL \u0026 SA\u00dc Graduated\n              Bursa \u2708\ufe0f Berlin\n                    Archer \n______________\ud83c\uddf9\ud83c\uddf7_____________","blocked_by_viewer":false,"country_block":false,"external_url":null,"external_url_linkshimmed":null,"edge_followed_by":{"count":547},"followed_by_viewer":false,"edge_follow":{"count":299},"follows_viewer":false,"full_name":"____________\u003cTK\u003e____________","has_blocked_viewer":false,"has_requested_viewer":false,"id":"1700499581","is_private":true,"is_verified":false,"mutual_followers":null,"profile_pic_url":"https://scontent-frx5-1.cdninstagram.com/vp/ae8cca32468cae276fd70a823898fcc1/5B28BE4A/t51.2885-19/s150x150/26866731_836251886546942_8991696596055883776_n.jpg","profile_pic_url_hd":"https://scontent-frx5-1.cdninstagram.com/vp/e53ac13652c0e170cd623c31c3e73385/5B18ABBA/t51.2885-19/s320x320/26866731_836251886546942_8991696596055883776_n.jpg","requested_by_viewer":false,"username":"tlgkyck","connected_fb_page":null,"edge_owner_to_timeline_media":{"count":209,"page_info":{"has_next_page":true,"end_cursor":"AQBpSHsXYn5mziP8mUv7z1JpUTbTwVNpTaqwngX03qrhG0LFkcmgQzDd9XQZ83SZZ7VWJs3UYQbYzjJzg6pQcnpS6J9KCbtoAaee8jYyHwyrkA"},"edges":[]},"edge_saved_media":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]},"edge_media_collections":{"count":0,"page_info":{"has_next_page":false,"end_cursor":null},"edges":[]}}}}]},"gatekeepers":{"ld":true,"seo":true},"qe":{"834cfd9a":{"g":"","p":{}},"client_gql":{"g":"","p":{}},"b57bc793":{"g":"","p":{}},"dash_for_vod":{"g":"","p":{}},"f6b232bb":{"g":"","p":{}},"bc3l":{"g":"","p":{}},"a47f578c":{"g":"","p":{}},"aysf":{"g":"","p":{}},"04eaabb0":{"g":"","p":{}},"notif":{"g":"","p":{}},"25b356ab":{"g":"","p":{}},"follow_button":{"g":"","p":{}},"e2cffd31":{"g":"test","p":{"new_cta":"true","remove_upsell_banner":"true","update_nav":"true"}},"loggedout":{"g":"test","p":{"new_cta":"true","remove_upsell_banner":"true","update_nav":"true"}},"8a5c80fd":{"g":"","p":{}},"loggedout_upsell":{"g":"","p":{}},"bd6730a0":{"g":"","p":{}},"stories":{"g":"","p":{}},"76a86dfb":{"g":"","p":{}},"exit_story_creation":{"g":"","p":{}},"df78c718":{"g":"test_msisdn_prefill_12_18","p":{"has_msisdn_prefill":"true"}},"su_universe":{"g":"test_msisdn_prefill_12_18","p":{"has_msisdn_prefill":"true"}},"11bbbc09":{"g":"","p":{}},"us_li":{"g":"","p":{}},"d16c94c5":{"g":"","p":{}},"sidecar":{"g":"","p":{}},"af886adf":{"g":"","p":{}},"video":{"g":"","p":{}},"bb21ed8b":{"g":"","p":{}},"appsell":{"g":"","p":{}},"78e2146b":{"g":"","p":{}},"collections":{"g":"","p":{}},"47d6a3b3":{"g":"control_prefill_2_15","p":{"has_msisdn_prefill":"false"}},"msisdn":{"g":"control_prefill_2_15","p":{"has_msisdn_prefill":"false"}},"4ae576c1":{"g":"","p":{}},"save":{"g":"","p":{}},"9dcf4750":{"g":"","p":{}},"stale":{"g":"","p":{}},"edc7f6d2":{"g":"new_reg_with_appsells_01_10","p":{"has_new_landing_appsells":"true","has_new_landing_page":"true"}},"reg":{"g":"new_reg_with_appsells_01_10","p":{"has_new_landing_appsells":"true","has_new_landing_page":"true"}},"47ce4b24":{"g":"control_group_1","p":{"hide_value_prop":"false"}},"reg_vp":{"g":"control_group_1","p":{"hide_value_prop":"false"}},"1df00ebb":{"g":"","p":{}},"prof_pic_upsell":{"g":"","p":{}},"004e9939":{"g":"","p":{}},"prof_pic_creation":{"g":"","p":{}},"fbce4ce4":{"g":"","p":{}},"onetaplogin":{"g":"","p":{}},"b239bf2d":{"g":"","p":{}},"onetaplogin_userbased":{"g":"","p":{}},"6bf718a8":{"g":"","p":{}},"feed_vp":{"g":"","p":{}},"8365e413":{"g":"","p":{}},"push_notifications":{"g":"","p":{}},"94df4b40":{"g":"","p":{}},"login_poe":{"g":"","p":{}},"4844df36":{"g":"","p":{}},"report_haf":{"g":"","p":{}},"f4651ae9":{"g":"","p":{}},"report_profile":{"g":"","p":{}},"47d2aebf":{"g":"","p":{}},"reporting":{"g":"","p":{}},"cb1ff25c":{"g":"","p":{}},"media_reporting":{"g":"","p":{}},"0d3bf783":{"g":"","p":{}},"bg_sync":{"g":"","p":{}},"ea55ef64":{"g":"","p":{}},"disc_ppl":{"g":"","p":{}},"28cc279b":{"g":"","p":{}},"ebdsim_li":{"g":"","p":{}},"3c0bc5c7":{"g":"","p":{}},"ebdsim_lo":{"g":"","p":{}},"d5dde92a":{"g":"","p":{}},"embeds":{"g":"","p":{}},"ca7fa6dd":{"g":"","p":{}},"prvcy_tggl":{"g":"","p":{}},"608b2c6c":{"g":"","p":{}},"tp_pblshr":{"g":"","p":{}},"2ea1c751":{"g":"","p":{}},"fs":{"g":"","p":{}},"b212f68e":{"g":"","p":{}},"404_as_react":{"g":"","p":{}},"d8c67ea6":{"g":"","p":{}},"acc_recovery":{"g":"","p":{}},"e878cb91":{"g":"","p":{}},"connections":{"g":"","p":{}},"0370381b":{"g":"","p":{}},"notif_banner":{"g":"","p":{}},"3b5f1021":{"g":"","p":{}},"private_lo":{"g":"","p":{}}},"hostname":"www.instagram.com","display_properties_server_guess":{"pixel_ratio":1.5,"viewport_width":360,"viewport_height":480,"orientation":""},"environment_switcher_visible_server_guess":true,"platform":"web","nonce":"pPj5YFbXoKZSZI1XCnJ8eQ==","zero_data":{},"rollout_hash":"3156f3856bb5","probably_has_app":false,"show_app_install":true};
+!function(e){function a(n){if(o[n])return o[n].exports;var t=o[n]={i:n,l:!1,exports:{}};return e[n].call(t.exports,t,t.exports,a),t.l=!0,t.exports}var n=window.webpackJsonp;window.webpackJsonp=function(o,r,i){for(var c,d,s,g=0,f=[];g&lt;o.length;g++)d=o[g],t[d]&amp;&amp;f.push(t[d][0]),t[d]=0;for(c in r)Object.prototype.hasOwnProperty.call(r,c)&amp;&amp;(e[c]=r[c]);for(n&amp;&amp;n(o,r,i);f.length;)f.shift()();if(i)for(g=0;g&lt;i.length;g++)s=a(a.s=i[g]);return s};var o={},t={49:0};a.e=function(e){function n(){c.onerror=c.onload=null,clearTimeout(d);var a=t[e];0!==a&amp;&amp;(a&amp;&amp;a[1](new Error("Loading chunk "+e+" failed.")),t[e]=void 0)}var o=t[e];if(0===o)return new Promise(function(e){e()});if(o)return o[2];var r=new Promise(function(a,n){o=t[e]=[a,n]});o[2]=r;var i=document.getElementsByTagName("head")[0],c=document.createElement("script");c.type="text/javascript",c.charset="utf-8",c.async=!0,c.timeout=12e4,c.crossOrigin="anonymous",a.nc&amp;&amp;c.setAttribute("nonce",a.nc),c.src=a.p+""+({0:"SettingsModules",1:"ProfilePageContainer",2:"LikedByListContainer",3:"FollowListContainer",4:"CreationModules",5:"LocationPageContainer",6:"DiscoverMediaPageContainer",7:"DiscoverEmbedsPageContainer",8:"UserCollectionMediaPageContainer",9:"TagPageContainer",10:"DebugInfoNub",11:"FeedPageContainer",12:"LandingPage",13:"PostPageContainer",14:"LoginAndSignupPage",15:"ResetPasswordPageContainer",16:"UserCollectionsPageContainer",17:"MobileStoriesPage",18:"DesktopStoriesPage",19:"DiscoverPeoplePageContainer",20:"MultiStepSignupPage",21:"ContactHistoryPage",22:"LocationsDirectoryLandingPage",23:"LocationsDirectoryCountryPage",24:"LocationsDirectoryCityPage",25:"EmailConfirmationPage",26:"SuggestedDirectoryLandingPage",27:"ProfilesDirectoryLandingPage",28:"DirectoryPage",29:"HttpErrorPage",30:"ActivityFeedPage",31:"CameraPage",32:"StoryCreationPage",33:"NewUserInterstitial",34:"FBSignupPage",35:"ContactInvitesOptOutPage",36:"Report",37:"Copyright",38:"SupportInfo",39:"Community",40:"GenericSurvey",41:"Challenge",42:"Consumer",43:"EmailSnoozePage",44:"EmailUnsubscribePage",45:"ConfirmFollowDialog",46:"NotificationLandingPage"}[e]||e)+".js/"+{0:"34ea21d19385",1:"88a1a465402e",2:"2342482c75ef",3:"b9dcacbeebc8",4:"c1984d97bc70",5:"288026a6de18",6:"109f6d734863",7:"9e82b7c6ea0b",8:"c9e9bb9efe11",9:"92c450f75f4b",10:"1197ccc46117",11:"3dfd8fa6cfd8",12:"12285bb0b069",13:"27c91aa59fdd",14:"d0a40e755e1e",15:"dd787adc92eb",16:"a4a16427cde3",17:"5800bb273aaa",18:"0703aab3b464",19:"90a8b57ae564",20:"41fa98f6895a",21:"5e044281585c",22:"6858feeb0a66",23:"d1c754295774",24:"7ea767ae76ee",25:"923742376262",26:"d5d5986f3842",27:"1352aea86cc0",28:"bd34aef749f3",29:"762c22ea65a3",30:"d366074da593",31:"ac0ef7598973",32:"fec058817877",33:"e037bebe8036",34:"6c4311554b3b",35:"95a47539d8b2",36:"494c93e40323",37:"5f29e1fddd91",38:"d9582b7fd06a",39:"3c182b8237da",40:"66ae1b2c8d3e",41:"ff6fd0e21ca6",42:"3034c2271934",43:"ba7e7b31317a",44:"a77601a12715",45:"b4a125eea937",46:"30463ebe552b"}[e]+".js";var d=setTimeout(n,12e4);return c.onerror=c.onload=n,i.appendChild(c),r},a.m=e,a.c=o,a.d=function(e,n,o){a.o(e,n)||Object.defineProperty(e,n,{configurable:!1,enumerable:!0,get:o})},a.n=function(e){var n=e&amp;&amp;e.__esModule?function(){return e.default}:function(){return e};return a.d(n,"a",n),n},a.o=function(e,a){return Object.prototype.hasOwnProperty.call(e,a)},a.p="/static/bundles/",a.oe=function(e){throw console.error(e),e}}([]);
+!function(f,b,e,v,n,t,s){if(f.fbq)return;n=f.fbq=function(){n.callMethod?
+n.callMethod.apply(n,arguments):n.queue.push(arguments)};if(!f._fbq)f._fbq=n;
+n.push=n;n.loaded=!0;n.version='2.0';n.queue=[];t=b.createElement(e);t.async=!0;
+t.src=v;s=b.getElementsByTagName(e)[0];s.parentNode.insertBefore(t,s)}(window,
+document,'script','//connect.facebook.net/en_US/fbevents.js');
+fbq('init', '1425767024389221');
+fbq('track', 'PageView');
+</t>
   </si>
 </sst>
 </file>
@@ -1233,7 +1285,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z57"/>
+  <dimension ref="A1:Z61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
@@ -1874,6 +1926,50 @@
         <v>60</v>
       </c>
     </row>
+    <row r="58" spans="1:26">
+      <c r="A58" s="2" t="n">
+        <v>43157.68808412573</v>
+      </c>
+      <c r="C58" t="s">
+        <v>61</v>
+      </c>
+      <c r="I58" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26">
+      <c r="A59" s="2" t="n">
+        <v>43157.68838307775</v>
+      </c>
+      <c r="C59" t="s">
+        <v>62</v>
+      </c>
+      <c r="I59" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26">
+      <c r="A60" s="2" t="n">
+        <v>43158.07107937009</v>
+      </c>
+      <c r="C60" t="s">
+        <v>63</v>
+      </c>
+      <c r="I60" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26">
+      <c r="A61" s="2" t="n">
+        <v>43158.07469307163</v>
+      </c>
+      <c r="C61" t="s">
+        <v>64</v>
+      </c>
+      <c r="I61" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>